<commit_message>
chore: publish terminology IG 2.0.0
</commit_message>
<xml_diff>
--- a/ig/terminology/CodeSystem-medcom-careCommunication-categoryCodes.xlsx
+++ b/ig/terminology/CodeSystem-medcom-careCommunication-categoryCodes.xlsx
@@ -7,13 +7,14 @@
   </bookViews>
   <sheets>
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
-    <sheet name="Concepts" r:id="rId4" sheetId="2"/>
+    <sheet name="Properties" r:id="rId4" sheetId="2"/>
+    <sheet name="Concepts" r:id="rId5" sheetId="3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="87">
   <si>
     <t>Property</t>
   </si>
@@ -30,7 +31,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.8.1</t>
+    <t>1.0.2</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +61,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-11-01</t>
+    <t>2025-09-22</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -120,15 +121,45 @@
     <t>Count</t>
   </si>
   <si>
-    <t>16</t>
+    <t>18</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Uri</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/concept-properties#status</t>
+  </si>
+  <si>
+    <t>A property that indicates the status of the concept. One of active, experimental, deprecated, or retired.</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>effectiveDate</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/concept-properties#effectiveDate</t>
+  </si>
+  <si>
+    <t>The date at which the concept status was last changed.</t>
+  </si>
+  <si>
+    <t>dateTime</t>
   </si>
   <si>
     <t>Level</t>
   </si>
   <si>
-    <t>Code</t>
-  </si>
-  <si>
     <t>Display</t>
   </si>
   <si>
@@ -226,6 +257,18 @@
   </si>
   <si>
     <t>Training</t>
+  </si>
+  <si>
+    <t>acute-ambulant</t>
+  </si>
+  <si>
+    <t>Acute ambulant</t>
+  </si>
+  <si>
+    <t>extended-care-responsibility</t>
+  </si>
+  <si>
+    <t>Extended care responsibility</t>
   </si>
   <si>
     <t>other</t>
@@ -544,7 +587,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -558,203 +601,282 @@
         <v>37</v>
       </c>
       <c r="C1" t="s" s="1">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s" s="1">
         <v>38</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>39</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s" s="2">
         <v>40</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="C2" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="C2" t="s" s="2">
+      <c r="D2" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="D2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s" s="2">
+        <v>54</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s" s="2">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C8" t="s" s="2">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="D8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="C9" t="s" s="2">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C10" t="s" s="2">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="D10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s" s="2">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D11" s="2"/>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s" s="2">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="D12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C13" t="s" s="2">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="D13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C14" t="s" s="2">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="D14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="C15" t="s" s="2">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="D15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C16" t="s" s="2">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="D16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="C17" t="s" s="2">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="D17" s="2"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="C18" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="C19" t="s" s="2">
+        <v>86</v>
+      </c>
+      <c r="D19" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
chore: publish terminology IG 2.0.0 (#33)
Co-authored-by: olw-medcom <olw-medcom@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ig/terminology/CodeSystem-medcom-careCommunication-categoryCodes.xlsx
+++ b/ig/terminology/CodeSystem-medcom-careCommunication-categoryCodes.xlsx
@@ -7,13 +7,14 @@
   </bookViews>
   <sheets>
     <sheet name="Metadata" r:id="rId3" sheetId="1"/>
-    <sheet name="Concepts" r:id="rId4" sheetId="2"/>
+    <sheet name="Properties" r:id="rId4" sheetId="2"/>
+    <sheet name="Concepts" r:id="rId5" sheetId="3"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="87">
   <si>
     <t>Property</t>
   </si>
@@ -30,7 +31,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.8.1</t>
+    <t>1.0.2</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +61,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2022-11-01</t>
+    <t>2025-09-22</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -120,15 +121,45 @@
     <t>Count</t>
   </si>
   <si>
-    <t>16</t>
+    <t>18</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Uri</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>status</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/concept-properties#status</t>
+  </si>
+  <si>
+    <t>A property that indicates the status of the concept. One of active, experimental, deprecated, or retired.</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>effectiveDate</t>
+  </si>
+  <si>
+    <t>http://hl7.org/fhir/concept-properties#effectiveDate</t>
+  </si>
+  <si>
+    <t>The date at which the concept status was last changed.</t>
+  </si>
+  <si>
+    <t>dateTime</t>
   </si>
   <si>
     <t>Level</t>
   </si>
   <si>
-    <t>Code</t>
-  </si>
-  <si>
     <t>Display</t>
   </si>
   <si>
@@ -226,6 +257,18 @@
   </si>
   <si>
     <t>Training</t>
+  </si>
+  <si>
+    <t>acute-ambulant</t>
+  </si>
+  <si>
+    <t>Acute ambulant</t>
+  </si>
+  <si>
+    <t>extended-care-responsibility</t>
+  </si>
+  <si>
+    <t>Extended care responsibility</t>
   </si>
   <si>
     <t>other</t>
@@ -544,7 +587,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -558,203 +601,282 @@
         <v>37</v>
       </c>
       <c r="C1" t="s" s="1">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s" s="1">
         <v>38</v>
-      </c>
-      <c r="D1" t="s" s="1">
-        <v>39</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="2">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s" s="2">
         <v>40</v>
       </c>
-      <c r="B2" t="s" s="2">
+      <c r="C2" t="s" s="2">
         <v>41</v>
       </c>
-      <c r="C2" t="s" s="2">
+      <c r="D2" t="s" s="2">
         <v>42</v>
       </c>
-      <c r="D2" s="2"/>
     </row>
     <row r="3">
       <c r="A3" t="s" s="2">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>44</v>
+        <v>45</v>
+      </c>
+      <c r="D3" t="s" s="2">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1:D19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s" s="1">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>36</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>48</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s" s="2">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s" s="2">
+        <v>52</v>
+      </c>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="B3" t="s" s="2">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s" s="2">
+        <v>54</v>
       </c>
       <c r="D3" s="2"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5">
       <c r="A5" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="D5" s="2"/>
     </row>
     <row r="6">
       <c r="A6" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7">
       <c r="A7" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B7" t="s" s="2">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="C7" t="s" s="2">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="D7" s="2"/>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="C8" t="s" s="2">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="D8" s="2"/>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="C9" t="s" s="2">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="D9" s="2"/>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="C10" t="s" s="2">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="D10" s="2"/>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s" s="2">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D11" s="2"/>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B12" t="s" s="2">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="C12" t="s" s="2">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="D12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="C13" t="s" s="2">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="D13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C14" t="s" s="2">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="D14" s="2"/>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="C15" t="s" s="2">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="D15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C16" t="s" s="2">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="D16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>71</v>
+        <v>81</v>
       </c>
       <c r="C17" t="s" s="2">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="D17" s="2"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="B18" t="s" s="2">
+        <v>83</v>
+      </c>
+      <c r="C18" t="s" s="2">
+        <v>84</v>
+      </c>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="s" s="2">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s" s="2">
+        <v>85</v>
+      </c>
+      <c r="C19" t="s" s="2">
+        <v>86</v>
+      </c>
+      <c r="D19" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>

<commit_message>
chore: publish terminology IG 2.0.1
</commit_message>
<xml_diff>
--- a/ig/terminology/CodeSystem-medcom-careCommunication-categoryCodes.xlsx
+++ b/ig/terminology/CodeSystem-medcom-careCommunication-categoryCodes.xlsx
@@ -31,7 +31,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.2</t>
+    <t>1.9.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -61,7 +61,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-09-22</t>
+    <t>2025-10-28</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
chore: publish terminology IG 2.0.1 (#46)
Co-authored-by: olw-medcom <olw-medcom@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/ig/terminology/CodeSystem-medcom-careCommunication-categoryCodes.xlsx
+++ b/ig/terminology/CodeSystem-medcom-careCommunication-categoryCodes.xlsx
@@ -31,7 +31,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.2</t>
+    <t>1.9.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -61,7 +61,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-09-22</t>
+    <t>2025-10-28</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>